<commit_message>
Landing page wrongly redirected issue fixed, changed to popular in community
</commit_message>
<xml_diff>
--- a/Src/VzMach/VzMach/App_Data/Data.xlsx
+++ b/Src/VzMach/VzMach/App_Data/Data.xlsx
@@ -45,7 +45,7 @@
     <t>B0003, B0004</t>
   </si>
   <si>
-    <t>B00013,B00032</t>
+    <t>B0013,B0032</t>
   </si>
   <si>
     <t>B0001,B0020,B0031</t>
@@ -434,22 +434,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
     <font>
@@ -497,19 +492,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -517,7 +512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
@@ -865,14 +860,16 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="8.45714285714286" style="4" customWidth="1"/>
     <col min="2" max="2" width="5.54285714285714" customWidth="1"/>
-    <col min="3" max="5" width="12.7238095238095" customWidth="1"/>
+    <col min="3" max="3" width="12.7238095238095" customWidth="1"/>
+    <col min="4" max="4" width="19.2857142857143" customWidth="1"/>
+    <col min="5" max="5" width="12.7238095238095" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="8" max="8" width="9.26666666666667" customWidth="1"/>
   </cols>

</xml_diff>